<commit_message>
Ajout du .xlsx et de la fig 3
</commit_message>
<xml_diff>
--- a/lab7/lab7.xlsx
+++ b/lab7/lab7.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Chart2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Chart3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
@@ -18,32 +19,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
-  <si>
-    <t>#3</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>#4</t>
-  </si>
-  <si>
-    <t>-56.5db</t>
-  </si>
-  <si>
-    <t>#5</t>
-  </si>
-  <si>
-    <t>swr</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -148,6 +123,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -764,6 +740,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="182003968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -806,8 +792,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.46384481953963E-2"/>
-              <c:y val="1.58491595044086E-2"/>
+              <c:x val="5.8553792781585248E-3"/>
+              <c:y val="0.11663847475767312"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -816,6 +802,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="182003392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -823,6 +819,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1496,6 +1493,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="182007424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -1555,12 +1562,773 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="182006848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
         </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Impédance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> intrinsèque en fonction de la fréquence pour différents modes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Mode (1,0)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$AA$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$AA$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1082.39779669205</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>659.01880520278996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>550.82070044212003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>499.59260170425199</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>469.72285545323598</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>450.27887296303498</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>436.71221902586899</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>426.778620213225</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>419.24057930765798</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>413.35982397423999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>408.66913556051401</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>404.85890634185603</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>401.71624042119299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>399.09021963017199</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>396.87109451539601</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>394.97729919337701</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>393.34706500713202</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>391.93284256383799</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>390.69749593121401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mode (2,0)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$AA$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$AA$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1082.39779669205</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>778.41012510718599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>659.01880520278996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>593.07662679300404</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>550.82070044212003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>521.33863756906703</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>499.59260170425199</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>482.90782614236502</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>469.72285545323598</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>459.06110507147702</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>450.27887296303498</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>442.93395294650401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Mode (0,1)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$AA$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2132.7001669208198</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>978.12311438826396</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>760.44336609641095</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>659.01880520278996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>598.93562503678697</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>558.85467747225402</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>530.12490807384404</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>508.50831562594902</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>491.66294444146001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>478.18108040298802</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>467.16222111979903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="81598080"/>
+        <c:axId val="78856768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81598080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Fréquence (GHz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.87863135811488124"/>
+              <c:y val="0.89863023352487537"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78856768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="78856768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Impédance</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> intrinsèque</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0">
+                    <a:sym typeface="Symbol"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="81598080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1607,6 +2375,17 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Chart3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
@@ -1635,6 +2414,33 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8675783" cy="6300271"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -1984,15 +2790,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AA38"/>
+  <dimension ref="B1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -2072,7 +2878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
@@ -2152,7 +2958,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -2232,7 +3038,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -2312,7 +3118,7 @@
         <v>1.49E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0</v>
       </c>
@@ -2392,7 +3198,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0</v>
       </c>
@@ -2472,7 +3278,7 @@
         <v>289482275.10501403</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
@@ -2552,7 +3358,7 @@
         <v>255342809.57156599</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0</v>
       </c>
@@ -2632,7 +3438,87 @@
         <v>242100056.2265</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11">
+        <v>12</v>
+      </c>
+      <c r="O11">
+        <v>13</v>
+      </c>
+      <c r="P11">
+        <v>14</v>
+      </c>
+      <c r="Q11">
+        <v>15</v>
+      </c>
+      <c r="R11">
+        <v>16</v>
+      </c>
+      <c r="S11">
+        <v>17</v>
+      </c>
+      <c r="T11">
+        <v>18</v>
+      </c>
+      <c r="U11">
+        <v>19</v>
+      </c>
+      <c r="V11">
+        <v>20</v>
+      </c>
+      <c r="W11">
+        <v>21</v>
+      </c>
+      <c r="X11">
+        <v>22</v>
+      </c>
+      <c r="Y11">
+        <v>23</v>
+      </c>
+      <c r="Z11">
+        <v>24</v>
+      </c>
+      <c r="AA11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0</v>
       </c>
@@ -2712,7 +3598,7 @@
         <v>390.69749593121401</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0</v>
       </c>
@@ -2792,7 +3678,7 @@
         <v>442.93395294650401</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0</v>
       </c>
@@ -2870,140 +3756,6 @@
       </c>
       <c r="AA14">
         <v>467.16222111979903</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>54.1</v>
-      </c>
-      <c r="C18">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>72.5</v>
-      </c>
-      <c r="C19">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>92</v>
-      </c>
-      <c r="C20">
-        <v>16.2</v>
-      </c>
-      <c r="D20">
-        <v>18.033333330000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>108.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>50.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>95</v>
-      </c>
-      <c r="B30">
-        <v>-56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>77.8</v>
-      </c>
-      <c r="B31">
-        <v>-56.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>58.7</v>
-      </c>
-      <c r="B32">
-        <v>-56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>42</v>
-      </c>
-      <c r="B33">
-        <v>-56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>104.9</v>
-      </c>
-      <c r="B36">
-        <v>-53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>86.7</v>
-      </c>
-      <c r="B37">
-        <v>-53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>50</v>
-      </c>
-      <c r="B38">
-        <v>-53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout du projet 3
</commit_message>
<xml_diff>
--- a/lab7/lab7.xlsx
+++ b/lab7/lab7.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>#3</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>$\lambda_g$</t>
+  </si>
+  <si>
+    <t>$\lambda_{gMOY}$</t>
+  </si>
+  <si>
+    <t>Données obtenues lors de la mesure de la longueur d'onde guidée $\lambda_g$</t>
   </si>
 </sst>
 </file>
@@ -721,11 +736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="174794432"/>
-        <c:axId val="174795008"/>
+        <c:axId val="177678016"/>
+        <c:axId val="177678592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="174794432"/>
+        <c:axId val="177678016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,12 +791,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174795008"/>
+        <c:crossAx val="177678592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174795008"/>
+        <c:axId val="177678592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -838,7 +853,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174794432"/>
+        <c:crossAx val="177678016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1479,11 +1494,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="174797888"/>
-        <c:axId val="174798464"/>
+        <c:axId val="177681472"/>
+        <c:axId val="177682048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="174797888"/>
+        <c:axId val="177681472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,12 +1544,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174798464"/>
+        <c:crossAx val="177682048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174798464"/>
+        <c:axId val="177682048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1598,7 +1613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174797888"/>
+        <c:crossAx val="177681472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1663,7 +1678,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2235,11 +2249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="174596096"/>
-        <c:axId val="174596672"/>
+        <c:axId val="177479680"/>
+        <c:axId val="177480256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="174596096"/>
+        <c:axId val="177479680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2286,12 +2300,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174596672"/>
+        <c:crossAx val="177480256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174596672"/>
+        <c:axId val="177480256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2335,7 +2349,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2352,14 +2365,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174596096"/>
+        <c:crossAx val="177479680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2818,8 +2830,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D38"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3789,28 +3801,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>54.1</v>
       </c>
       <c r="C18">
         <v>18.399999999999999</v>
       </c>
+      <c r="E18">
+        <f>C18*2</f>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>54.1</v>
+      </c>
+      <c r="J18">
+        <v>72.5</v>
+      </c>
+      <c r="K18">
+        <v>92</v>
+      </c>
+      <c r="L18">
+        <v>108.2</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>72.5</v>
       </c>
       <c r="C19">
         <v>19.5</v>
       </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E20" si="0">C19*2</f>
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J19">
+        <v>39</v>
+      </c>
+      <c r="K19">
+        <v>32.4</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>92</v>
       </c>
@@ -3820,33 +3876,46 @@
       <c r="D20">
         <v>18.033333330000001</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>32.4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>36.07</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>108.2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>50.6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -3854,7 +3923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>95</v>
       </c>
@@ -3862,7 +3931,7 @@
         <v>-56</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>77.8</v>
       </c>
@@ -3870,7 +3939,7 @@
         <v>-56.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>58.7</v>
       </c>

</xml_diff>

<commit_message>
Ajout des figures et des différents fichiers matlab et excel
</commit_message>
<xml_diff>
--- a/lab7/lab7.xlsx
+++ b/lab7/lab7.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500" activeTab="3"/>
@@ -12,7 +12,7 @@
     <sheet name="Chart3" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>#3</t>
   </si>
@@ -43,21 +43,6 @@
   </si>
   <si>
     <t>max</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>mm</t>
-  </si>
-  <si>
-    <t>$\lambda_g$</t>
-  </si>
-  <si>
-    <t>$\lambda_{gMOY}$</t>
-  </si>
-  <si>
-    <t>Données obtenues lors de la mesure de la longueur d'onde guidée $\lambda_g$</t>
   </si>
 </sst>
 </file>
@@ -106,17 +91,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -164,7 +157,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -189,82 +181,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,82 +268,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.123</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.5600000000000006E-2</c:v>
+                  <c:v>0.0656</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.87E-2</c:v>
+                  <c:v>0.0487</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9800000000000002E-2</c:v>
+                  <c:v>0.0398</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.4000000000000002E-2</c:v>
+                  <c:v>0.034</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9899999999999999E-2</c:v>
+                  <c:v>0.0299</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.6700000000000002E-2</c:v>
+                  <c:v>0.0267</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4299999999999999E-2</c:v>
+                  <c:v>0.0243</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2200000000000001E-2</c:v>
+                  <c:v>0.0222</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.06E-2</c:v>
+                  <c:v>0.0206</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.9099999999999999E-2</c:v>
+                  <c:v>0.0191</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.7899999999999999E-2</c:v>
+                  <c:v>0.0179</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.6799999999999999E-2</c:v>
+                  <c:v>0.0168</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.5900000000000001E-2</c:v>
+                  <c:v>0.0159</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.015</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.43E-2</c:v>
+                  <c:v>0.0143</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3599999999999999E-2</c:v>
+                  <c:v>0.0136</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2999999999999999E-2</c:v>
+                  <c:v>0.013</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.24E-2</c:v>
+                  <c:v>0.0124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,82 +366,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,82 +453,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.1499999999999999E-2</c:v>
+                  <c:v>0.0615</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.1300000000000003E-2</c:v>
+                  <c:v>0.0413</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2800000000000003E-2</c:v>
+                  <c:v>0.0328</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.7799999999999998E-2</c:v>
+                  <c:v>0.0278</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.4400000000000002E-2</c:v>
+                  <c:v>0.0244</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.18E-2</c:v>
+                  <c:v>0.0218</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9900000000000001E-2</c:v>
+                  <c:v>0.0199</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.83E-2</c:v>
+                  <c:v>0.0183</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>0.017</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5900000000000001E-2</c:v>
+                  <c:v>0.0159</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.49E-2</c:v>
+                  <c:v>0.0149</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.41E-2</c:v>
+                  <c:v>0.0141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,82 +551,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,82 +638,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.11310000000000001</c:v>
+                  <c:v>0.1131</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.8599999999999997E-2</c:v>
+                  <c:v>0.0486</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.56E-2</c:v>
+                  <c:v>0.0356</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.9100000000000001E-2</c:v>
+                  <c:v>0.0291</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5100000000000001E-2</c:v>
+                  <c:v>0.0251</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2200000000000001E-2</c:v>
+                  <c:v>0.0222</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.01E-2</c:v>
+                  <c:v>0.0201</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.84E-2</c:v>
+                  <c:v>0.0184</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.7000000000000001E-2</c:v>
+                  <c:v>0.017</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.5900000000000001E-2</c:v>
+                  <c:v>0.0159</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.49E-2</c:v>
+                  <c:v>0.0149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -736,11 +728,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177678016"/>
-        <c:axId val="177678592"/>
+        <c:axId val="584507128"/>
+        <c:axId val="584441800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177678016"/>
+        <c:axId val="584507128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,8 +763,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.83796932219259102"/>
-              <c:y val="0.87662371983681298"/>
+              <c:x val="0.837969322192591"/>
+              <c:y val="0.876623719836813"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -791,15 +783,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177678592"/>
+        <c:crossAx val="584441800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177678592"/>
+        <c:axId val="584441800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -833,8 +825,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.8553792781585248E-3"/>
-              <c:y val="0.11663847475767312"/>
+              <c:x val="0.00585537927815853"/>
+              <c:y val="0.116638474757673"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -853,14 +845,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177678016"/>
+        <c:crossAx val="584507128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -919,8 +910,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12846333293490625"/>
-          <c:y val="1.8142076745587609E-2"/>
+          <c:x val="0.128463332934906"/>
+          <c:y val="0.0181420767455876"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -947,82 +938,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1034,82 +1025,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>104490234.87081</c:v>
+                  <c:v>1.0449023487081E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>171618774.922815</c:v>
+                  <c:v>1.71618774922815E8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>205329973.81764999</c:v>
+                  <c:v>2.0532997381765E8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>226384457.284163</c:v>
+                  <c:v>2.26384457284163E8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>240780278.598259</c:v>
+                  <c:v>2.40780278598259E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>251177674.08395499</c:v>
+                  <c:v>2.51177674083955E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>258980617.14939201</c:v>
+                  <c:v>2.58980617149392E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>265008589.098239</c:v>
+                  <c:v>2.65008589098239E8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>269773503.764296</c:v>
+                  <c:v>2.69773503764296E8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>273611496.42604899</c:v>
+                  <c:v>2.73611496426049E8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>276751998.52045798</c:v>
+                  <c:v>2.76751998520458E8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>279356581.33824098</c:v>
+                  <c:v>2.79356581338241E8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>281542015.53170103</c:v>
+                  <c:v>2.81542015531701E8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>283394567.03501099</c:v>
+                  <c:v>2.83394567035011E8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>284979182.316369</c:v>
+                  <c:v>2.84979182316369E8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>286345570.31751698</c:v>
+                  <c:v>2.86345570317517E8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>287532334.82992798</c:v>
+                  <c:v>2.87532334829928E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>288569845.94644803</c:v>
+                  <c:v>2.88569845946448E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>289482275.10501403</c:v>
+                  <c:v>2.89482275105014E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1132,82 +1123,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1219,82 +1210,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104490234.87081</c:v>
+                  <c:v>1.0449023487081E8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>145296157.32378399</c:v>
+                  <c:v>1.45296157323784E8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>171618774.922815</c:v>
+                  <c:v>1.71618774922815E8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>190700484.373454</c:v>
+                  <c:v>1.90700484373454E8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>205329973.81764999</c:v>
+                  <c:v>2.0532997381765E8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>216941526.77302101</c:v>
+                  <c:v>2.16941526773021E8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>226384457.284163</c:v>
+                  <c:v>2.26384457284163E8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>234206185.68864799</c:v>
+                  <c:v>2.34206185688648E8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>240780278.598259</c:v>
+                  <c:v>2.40780278598259E8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>246372430.05457801</c:v>
+                  <c:v>2.46372430054578E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>251177674.08395499</c:v>
+                  <c:v>2.51177674083955E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>255342809.57156599</c:v>
+                  <c:v>2.55342809571566E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1317,82 +1308,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1404,82 +1395,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>53031364.536953598</c:v>
+                  <c:v>5.30313645369536E7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>115629615.879934</c:v>
+                  <c:v>1.15629615879934E8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>148729024.46447399</c:v>
+                  <c:v>1.48729024464474E8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>171618774.922815</c:v>
+                  <c:v>1.71618774922815E8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>188834985.38437</c:v>
+                  <c:v>1.8883498538437E8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>202378193.40004599</c:v>
+                  <c:v>2.02378193400046E8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>213345945.97891599</c:v>
+                  <c:v>2.13345945978916E8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>222415241.84472701</c:v>
+                  <c:v>2.22415241844727E8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230035639.81923401</c:v>
+                  <c:v>2.30035639819234E8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>236521277.47230101</c:v>
+                  <c:v>2.36521277472301E8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>242100056.2265</c:v>
+                  <c:v>2.421000562265E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1494,11 +1485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177681472"/>
-        <c:axId val="177682048"/>
+        <c:axId val="654978584"/>
+        <c:axId val="524395800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177681472"/>
+        <c:axId val="654978584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,8 +1515,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.8783313275585618"/>
-              <c:y val="0.90064601982994064"/>
+              <c:x val="0.878331327558562"/>
+              <c:y val="0.900646019829941"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1544,15 +1535,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177682048"/>
+        <c:crossAx val="524395800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177682048"/>
+        <c:axId val="524395800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1596,7 +1587,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1613,7 +1603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177681472"/>
+        <c:crossAx val="654978584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1623,7 +1613,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1702,82 +1691,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1789,82 +1778,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1082.39779669205</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>659.01880520278996</c:v>
+                  <c:v>659.01880520279</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>550.82070044212003</c:v>
+                  <c:v>550.82070044212</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>499.59260170425199</c:v>
+                  <c:v>499.592601704252</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>469.72285545323598</c:v>
+                  <c:v>469.722855453236</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>450.27887296303498</c:v>
+                  <c:v>450.278872963035</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>436.71221902586899</c:v>
+                  <c:v>436.712219025869</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>426.778620213225</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>419.24057930765798</c:v>
+                  <c:v>419.240579307658</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>413.35982397423999</c:v>
+                  <c:v>413.35982397424</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>408.66913556051401</c:v>
+                  <c:v>408.669135560514</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>404.85890634185603</c:v>
+                  <c:v>404.858906341856</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>401.71624042119299</c:v>
+                  <c:v>401.716240421193</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>399.09021963017199</c:v>
+                  <c:v>399.090219630172</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>396.87109451539601</c:v>
+                  <c:v>396.871094515396</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>394.97729919337701</c:v>
+                  <c:v>394.977299193377</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>393.34706500713202</c:v>
+                  <c:v>393.347065007132</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>391.93284256383799</c:v>
+                  <c:v>391.932842563838</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>390.69749593121401</c:v>
+                  <c:v>390.697495931214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1887,82 +1876,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1974,82 +1963,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1082.39779669205</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>778.41012510718599</c:v>
+                  <c:v>778.410125107186</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>659.01880520278996</c:v>
+                  <c:v>659.01880520279</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>593.07662679300404</c:v>
+                  <c:v>593.076626793004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>550.82070044212003</c:v>
+                  <c:v>550.82070044212</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>521.33863756906703</c:v>
+                  <c:v>521.338637569067</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>499.59260170425199</c:v>
+                  <c:v>499.592601704252</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>482.90782614236502</c:v>
+                  <c:v>482.907826142365</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>469.72285545323598</c:v>
+                  <c:v>469.722855453236</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>459.06110507147702</c:v>
+                  <c:v>459.061105071477</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>450.27887296303498</c:v>
+                  <c:v>450.278872963035</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>442.93395294650401</c:v>
+                  <c:v>442.933952946504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2072,82 +2061,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>17.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2159,82 +2148,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2132.7001669208198</c:v>
+                  <c:v>2132.70016692082</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>978.12311438826396</c:v>
+                  <c:v>978.123114388264</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>760.44336609641095</c:v>
+                  <c:v>760.443366096411</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>659.01880520278996</c:v>
+                  <c:v>659.01880520279</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>598.93562503678697</c:v>
+                  <c:v>598.935625036787</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>558.85467747225402</c:v>
+                  <c:v>558.854677472254</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>530.12490807384404</c:v>
+                  <c:v>530.124908073844</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>508.50831562594902</c:v>
+                  <c:v>508.508315625949</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>491.66294444146001</c:v>
+                  <c:v>491.66294444146</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>478.18108040298802</c:v>
+                  <c:v>478.181080402988</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>467.16222111979903</c:v>
+                  <c:v>467.162221119799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2249,14 +2238,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177479680"/>
-        <c:axId val="177480256"/>
+        <c:axId val="655075992"/>
+        <c:axId val="137384488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177479680"/>
+        <c:axId val="655075992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="25"/>
+          <c:max val="25.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2280,8 +2269,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.87863135811488124"/>
-              <c:y val="0.89863023352487537"/>
+              <c:x val="0.878631358114881"/>
+              <c:y val="0.898630233524876"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2300,15 +2289,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177480256"/>
+        <c:crossAx val="137384488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177480256"/>
+        <c:axId val="137384488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2365,7 +2354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177479680"/>
+        <c:crossAx val="655075992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2830,13 +2819,13 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="B1">
         <v>0</v>
       </c>
@@ -2916,7 +2905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27">
       <c r="B2">
         <v>0</v>
       </c>
@@ -2996,7 +2985,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27">
       <c r="B3">
         <v>0</v>
       </c>
@@ -3076,7 +3065,7 @@
         <v>1.41E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27">
       <c r="B4">
         <v>0</v>
       </c>
@@ -3156,7 +3145,7 @@
         <v>1.49E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27">
       <c r="B6">
         <v>0</v>
       </c>
@@ -3236,7 +3225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27">
       <c r="B7">
         <v>0</v>
       </c>
@@ -3316,7 +3305,7 @@
         <v>289482275.10501403</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27">
       <c r="B8">
         <v>0</v>
       </c>
@@ -3396,7 +3385,7 @@
         <v>255342809.57156599</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27">
       <c r="B9">
         <v>0</v>
       </c>
@@ -3476,7 +3465,7 @@
         <v>242100056.2265</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27">
       <c r="B11">
         <v>0</v>
       </c>
@@ -3556,7 +3545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27">
       <c r="B12">
         <v>0</v>
       </c>
@@ -3636,7 +3625,7 @@
         <v>390.69749593121401</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27">
       <c r="B13">
         <v>0</v>
       </c>
@@ -3716,7 +3705,7 @@
         <v>442.93395294650401</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27">
       <c r="B14">
         <v>0</v>
       </c>
@@ -3796,77 +3785,33 @@
         <v>467.16222111979903</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27">
       <c r="A16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>54.1</v>
       </c>
       <c r="C18">
         <v>18.399999999999999</v>
       </c>
-      <c r="E18">
-        <f>C18*2</f>
-        <v>36.799999999999997</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18">
-        <v>54.1</v>
-      </c>
-      <c r="J18">
-        <v>72.5</v>
-      </c>
-      <c r="K18">
-        <v>92</v>
-      </c>
-      <c r="L18">
-        <v>108.2</v>
-      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>72.5</v>
       </c>
       <c r="C19">
         <v>19.5</v>
       </c>
-      <c r="E19">
-        <f t="shared" ref="E19:E20" si="0">C19*2</f>
-        <v>39</v>
-      </c>
-      <c r="G19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="J19">
-        <v>39</v>
-      </c>
-      <c r="K19">
-        <v>32.4</v>
-      </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>92</v>
       </c>
@@ -3876,46 +3821,33 @@
       <c r="D20">
         <v>18.033333330000001</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>32.4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20">
-        <v>36.07</v>
-      </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>108.2</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>50.6</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -3923,31 +3855,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>95</v>
       </c>
       <c r="B30">
         <v>-56</v>
       </c>
+      <c r="C30">
+        <f>A30-A31</f>
+        <v>17.200000000000003</v>
+      </c>
+      <c r="D30">
+        <f>AVERAGE(C30:C32)</f>
+        <v>17.666666666666668</v>
+      </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>77.8</v>
       </c>
       <c r="B31">
         <v>-56.5</v>
       </c>
+      <c r="C31">
+        <f t="shared" ref="C31:C32" si="0">A31-A32</f>
+        <v>19.099999999999994</v>
+      </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>58.7</v>
       </c>
       <c r="B32">
         <v>-56</v>
       </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>16.700000000000003</v>
+      </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>42</v>
       </c>
@@ -3955,7 +3903,7 @@
         <v>-56</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -3963,7 +3911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>104.9</v>
       </c>
@@ -3971,7 +3919,7 @@
         <v>-53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>86.7</v>
       </c>
@@ -3979,7 +3927,7 @@
         <v>-53</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>50</v>
       </c>

</xml_diff>